<commit_message>
editted sample sql code filters
</commit_message>
<xml_diff>
--- a/text/Data-Extraction-Filters-Summary.xlsx
+++ b/text/Data-Extraction-Filters-Summary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>SQL Query</t>
   </si>
@@ -24,178 +24,157 @@
     <t>Filters</t>
   </si>
   <si>
-    <t>get-commercial-biology.sql</t>
-  </si>
-  <si>
     <t>GFBio</t>
   </si>
   <si>
     <t>filtered out TRIP_SUBTYPE_CODE 2,3 (research trips)</t>
   </si>
   <si>
-    <t>filtered for SPECIMEN_SEX_CODE 1,2 (sexed as male/female)</t>
-  </si>
-  <si>
     <t>filtered for SAMPLE_SOURCE_CODE 1 (unsorted samples)</t>
   </si>
   <si>
-    <t>filtered for USABILITY_CODE 0,1,2,6 (usable samples)</t>
-  </si>
-  <si>
-    <t>filtered for FE_PARENT_EVENT_ID null (to include data at only one level - some data also recorded in database at higher or lower level with separate fishing event ID's)</t>
-  </si>
-  <si>
-    <t>get-survey-biology.sql</t>
-  </si>
-  <si>
     <t>filtered for TRIP_SUBTYPE_CODE 2,3 (research trips)</t>
   </si>
   <si>
-    <t>get-cpue.sql</t>
-  </si>
-  <si>
     <t>filtered for YEAR(BEST_DATE) &gt;2012</t>
   </si>
   <si>
-    <t>filtered for FISHERY_SECTOR 'GROUNDFISH TRAWL'</t>
-  </si>
-  <si>
-    <t>filtered for (LANDED_ROUND_KG + TOTAL_RELEASED_ROUND_KG) &gt;0</t>
-  </si>
-  <si>
-    <t>get-landings.sql</t>
-  </si>
-  <si>
     <t>GFFOS.MERGED_CATCH</t>
   </si>
   <si>
     <t>Database or Database.Table</t>
   </si>
   <si>
-    <t>get-survey-boot</t>
-  </si>
-  <si>
     <t>Extracting commercial biological data</t>
   </si>
   <si>
     <t>Extracting survey biological data</t>
   </si>
   <si>
-    <t>Extracting commercial trawl catch per unit effort (kg/hr)</t>
-  </si>
-  <si>
-    <t>Extract commercial landings</t>
-  </si>
-  <si>
-    <t>Extract bootstrapped survey biomass index</t>
-  </si>
-  <si>
     <t>GFFOS.GF_D_</t>
   </si>
   <si>
     <t>OFFICIAL_CATCH</t>
   </si>
   <si>
-    <t>Assign maturity status</t>
-  </si>
-  <si>
-    <t>maturity_assignment.sql</t>
-  </si>
-  <si>
-    <t>designates maturity code at and above which a sample assessed following a given maturity convention is considered mature</t>
-  </si>
-  <si>
-    <t>aging_precision.sql</t>
-  </si>
-  <si>
     <t>Extract all age readings to determine aging precision</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Hart Code</t>
-  </si>
-  <si>
-    <t>SARA Status</t>
-  </si>
-  <si>
-    <t>COSEWIC Status</t>
-  </si>
-  <si>
-    <t>Current TAC</t>
-  </si>
-  <si>
-    <t>Scorpaenidae</t>
-  </si>
-  <si>
-    <t>Special Concern</t>
-  </si>
-  <si>
     <t>Rationale</t>
   </si>
   <si>
-    <t>To extract only those records with specimen sex recorded</t>
-  </si>
-  <si>
-    <t>To remove samples from incomplete surveys, when gear was damaged, or other sampling errors</t>
-  </si>
-  <si>
     <t>To extract only samples which were unsorted (some of which are discarded) to avoid sampling bias</t>
   </si>
   <si>
-    <t xml:space="preserve">filtered for FE_PARENT_EVENT_ID null </t>
-  </si>
-  <si>
-    <t>To extract data at only one level - some data are also recorded in the database at higher or lower levels with separate fishing event ID's</t>
-  </si>
-  <si>
     <t>To extract only commercial data</t>
   </si>
   <si>
     <t>To extract only research data</t>
   </si>
   <si>
-    <t>should be irrelevant for survey data…, but may have affected our data extraction - check</t>
-  </si>
-  <si>
-    <t>filtered for LAT between 47.8 and 55 and LON between -135 and -122</t>
-  </si>
-  <si>
-    <t>To remove erroneous location records</t>
-  </si>
-  <si>
-    <t>To extract data since the fishery footprint was initiated</t>
-  </si>
-  <si>
-    <t>To select only trawl fishery data</t>
-  </si>
-  <si>
-    <t>To select only fishing events which had a positive catch for a species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filtered for END_DATE &gt; START_DATE AND YEAR(START_DATE) = YEAR(END_DATE)  </t>
-  </si>
-  <si>
-    <t>To remove erroneous date records</t>
-  </si>
-  <si>
     <t>no filters</t>
   </si>
   <si>
     <t>To extract all landings and discards by fishery sector and gear</t>
   </si>
   <si>
-    <t xml:space="preserve">filter for ACTIVE_IND 1 </t>
-  </si>
-  <si>
     <t>To extract only active (useable) bootstrapped index records</t>
   </si>
   <si>
-    <t>filter for AGE_READING_TYPE_CODE 2 or 3</t>
-  </si>
-  <si>
     <t>To extract only those aged specimen records which were aged using the break and burn or break and bake methods</t>
+  </si>
+  <si>
+    <t>get-comm-samples.sql</t>
+  </si>
+  <si>
+    <t>get-surv-samples.sql</t>
+  </si>
+  <si>
+    <t>get-catch.sql</t>
+  </si>
+  <si>
+    <t>get-cpue-index.sql</t>
+  </si>
+  <si>
+    <t>get-surv-index</t>
+  </si>
+  <si>
+    <t>get-age-precision.sql</t>
+  </si>
+  <si>
+    <t>Extract spatial trawl cpue</t>
+  </si>
+  <si>
+    <t>filtered lat between 47.8 and 55, lon between -135 and -122</t>
+  </si>
+  <si>
+    <t>To remove erroneous lat/lon</t>
+  </si>
+  <si>
+    <t>To only include data since trawl footprint was initiated</t>
+  </si>
+  <si>
+    <t>To only include bottom trawl records</t>
+  </si>
+  <si>
+    <t>filtered for FISHERY_SECTOR "GROUNDFISH TRAWL"</t>
+  </si>
+  <si>
+    <t>filtered for SAMPLE_TYPE_CODES 1 and 2 (total and random samples)</t>
+  </si>
+  <si>
+    <t>filtered for FE_START_DATE IS NOT NULL</t>
+  </si>
+  <si>
+    <t>filtered for FE_END_DATE IS NOT NULL</t>
+  </si>
+  <si>
+    <t>To only include records with a valid start date</t>
+  </si>
+  <si>
+    <t>To only include records with a valid end date</t>
+  </si>
+  <si>
+    <t>get-cpue-spatial.sql</t>
+  </si>
+  <si>
+    <t>get-cpue-spatial-ll.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filtered for ACTIVE_IND 1 </t>
+  </si>
+  <si>
+    <t>filtered for AGE_READING_TYPE_CODE 2 or 3</t>
+  </si>
+  <si>
+    <t>filtered for LAT IS NOT NULL and LON IS NOT NULL</t>
+  </si>
+  <si>
+    <t>To include only records from longline geartypes</t>
+  </si>
+  <si>
+    <t>To include only records since RCA's were established</t>
+  </si>
+  <si>
+    <t>Extract spatial longline cpue</t>
+  </si>
+  <si>
+    <t>Extract commercial catch</t>
+  </si>
+  <si>
+    <t>filtered for years &gt;= 2008</t>
+  </si>
+  <si>
+    <t>Extract survey biomass index</t>
+  </si>
+  <si>
+    <t>filtered for GEAR IN ('HOOK AND LINE', 'LONGLINE',  'LONGLINE OR HOOK AND LINE'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracting commercial trawl catch per unit effort </t>
+  </si>
+  <si>
+    <t>To extract only samples which were unsorted to avoid sampling bias</t>
   </si>
 </sst>
 </file>
@@ -227,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -298,21 +277,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -347,12 +311,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -386,37 +350,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -720,294 +684,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E25"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>15</v>
+      <c r="A19" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>23</v>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>2</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1017,10 +988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,37 +1003,7 @@
     <col min="5" max="5" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
-        <v>442</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
+    <row r="1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>